<commit_message>
JavaDoc Kommentare erstellt und Testing sheet ausgefüllt
</commit_message>
<xml_diff>
--- a/Use Case based Testing.xlsx
+++ b/Use Case based Testing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\GitHub\SoftwareHeros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403F6D84-14FA-4738-9DEC-369DFDDF2214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0EEE55-0E17-4C3E-A7CC-057E858CBF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8F0B6F25-0A00-6E48-9C26-F9E73014E07C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -72,61 +72,109 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>Alternative Flow</t>
-  </si>
-  <si>
-    <t>Test database 1 (with some test bookings)</t>
-  </si>
-  <si>
-    <t>Test database 7 (fully booked)</t>
-  </si>
-  <si>
-    <t>System shows no rooms and provides link for booking</t>
-  </si>
-  <si>
-    <t>Extension 1</t>
-  </si>
-  <si>
-    <t>120 mins</t>
-  </si>
-  <si>
-    <t>H101 is shown</t>
-  </si>
-  <si>
-    <t>H101, H211, H311, H471 are shown</t>
-  </si>
-  <si>
-    <t>- 60 mins</t>
-  </si>
-  <si>
-    <t>An error message is shown</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Not yet implemented</t>
-  </si>
-  <si>
-    <t>System does not respond</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
     <t>Branch, Version</t>
   </si>
   <si>
-    <t>main, faa0d69</t>
-  </si>
-  <si>
-    <t>main, xdf881</t>
+    <t>Alternative Flow 1</t>
+  </si>
+  <si>
+    <t>Test database (mit bereits existierenden Usern)</t>
+  </si>
+  <si>
+    <t>Test database (mit existierendem User "admin")</t>
+  </si>
+  <si>
+    <t>Benutzername existiert bereits</t>
+  </si>
+  <si>
+    <t>admin als Benutzername dann abbrechen bei Fehlermeldung</t>
+  </si>
+  <si>
+    <t>Nach Meldung über existierenden User bricht der Benutzer ab</t>
+  </si>
+  <si>
+    <t>Benutzer landet wieder im Menü</t>
+  </si>
+  <si>
+    <t>Alternative Flow 2</t>
+  </si>
+  <si>
+    <t>Alternative Flow 3</t>
+  </si>
+  <si>
+    <t>Abbrechen bei Abfrage auf Benutzernamen und Passwort</t>
+  </si>
+  <si>
+    <t>Benutzer bricht bei Registriervorgang ab</t>
+  </si>
+  <si>
+    <t>1, Register</t>
+  </si>
+  <si>
+    <t>10, Login</t>
+  </si>
+  <si>
+    <t>Erfolgsmeldung über Anmeldung und zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Benutzer gibt einmal falsche Anmeldedaten ein und die korrekten</t>
+  </si>
+  <si>
+    <t>Meldung über falsche Daten, erneute Dateneingabe, Erfolgsmeldung, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Benutzer bricht bei Anmeldevorgang ab</t>
+  </si>
+  <si>
+    <t>Test database (ohne User "Admin")</t>
+  </si>
+  <si>
+    <t>Benutzername und Passwort Admin, bei Fehlermeldung abbrechen</t>
+  </si>
+  <si>
+    <t>Fehlermeldung: falsche Anmeldedaten und bei Abbrechen zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Benutzer bricht nach falschen Anmeldedaten ab</t>
+  </si>
+  <si>
+    <t>Test database (mit existierendem User "admin" ohne "Mustermann")</t>
+  </si>
+  <si>
+    <t>Test database (ohne User "Max")</t>
+  </si>
+  <si>
+    <t>Erfolgsmeldung mit Benutzername und Passwort, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Fehlermeldung: der Benutzer existiert bereits und Abfrage nach neuem Benutzernamen, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Fehlermeldung: Benutzer existiert bereits, zurück zum Menü</t>
+  </si>
+  <si>
+    <t>Max als Benutzername, Meldung mit ok bestätigen</t>
+  </si>
+  <si>
+    <t>Benutzername und Passwort admin, Meldung mit ok bestätigen</t>
+  </si>
+  <si>
+    <t>Kierstein</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>admin als Benutzername bei erster Abfrage, Meldung mit ok bestätigen, Mustermann bei erneuter Abfrage</t>
+  </si>
+  <si>
+    <t>Admin bei erster Abfrage, Meldung mit ok bestätigen, admin bei zweiter Abfrage, Meldung mit ok bestätigen</t>
   </si>
 </sst>
 </file>
@@ -517,23 +565,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EFA617-FEF3-1540-8735-957D00343B99}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.125" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="92.375" customWidth="1"/>
     <col min="5" max="5" width="22.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="34.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,138 +601,219 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>26</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -730,15 +860,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E44AE7-7B0E-454D-A297-BCD6EF9884C1}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -755,10 +886,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -775,22 +906,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>44722</v>
+        <v>45103</v>
       </c>
       <c r="B2" s="6">
-        <v>0.33680555555555558</v>
+        <v>0.49444444444444446</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -798,22 +929,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>44722</v>
+        <v>45103</v>
       </c>
       <c r="B3" s="6">
-        <v>0.34027777777777773</v>
+        <v>0.49513888888888885</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -821,75 +952,144 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>44722</v>
+        <v>45103</v>
       </c>
       <c r="B4" s="6">
-        <v>0.34375</v>
+        <v>0.49652777777777773</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>44722</v>
+        <v>45103</v>
       </c>
       <c r="B5" s="6">
-        <v>0.34722222222222199</v>
+        <v>0.49722222222222223</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>44727</v>
+        <v>45103</v>
       </c>
       <c r="B6" s="6">
-        <v>0.35069444444444398</v>
+        <v>0.49791666666666662</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.49861111111111112</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>45103</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="F1:F1048576 G4 G9">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
     </cfRule>

</xml_diff>